<commit_message>
update all and phd of dean
</commit_message>
<xml_diff>
--- a/COSC 60 - IT 2D/POINTS - IT 2D.xlsx
+++ b/COSC 60 - IT 2D/POINTS - IT 2D.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\WORK\CvSU\2017-2018 Second Semester\Grading-Sheets-Second-Sem-2017-2018\COSC 60 - IT 2D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB08D50-5377-4184-8ABF-AA6122F14E55}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC4161B-3705-4342-84C3-604BC358784F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="135" windowWidth="20055" windowHeight="7185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="241">
   <si>
     <t>C</t>
   </si>
@@ -737,6 +737,15 @@
   </si>
   <si>
     <t>Kimberly</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Excess</t>
+  </si>
+  <si>
+    <t>Items</t>
   </si>
 </sst>
 </file>
@@ -1072,7 +1081,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1273,6 +1282,9 @@
     <xf numFmtId="0" fontId="1" fillId="24" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="60% - Accent1" xfId="2" builtinId="32"/>
@@ -1838,11 +1850,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN61"/>
+  <dimension ref="A1:AQ62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="AG1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AL10" sqref="AL10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <pane xSplit="5" topLeftCell="AM1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AN58" sqref="AN58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1855,7 +1867,7 @@
     <col min="38" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="15">
+    <row r="1" spans="1:43" ht="15">
       <c r="A1" s="57" t="s">
         <v>48</v>
       </c>
@@ -1906,8 +1918,15 @@
       <c r="AL1" s="56"/>
       <c r="AM1" s="56"/>
       <c r="AN1" s="56"/>
-    </row>
-    <row r="2" spans="1:40" ht="15">
+      <c r="AO1" s="73" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP1" s="73">
+        <v>80</v>
+      </c>
+      <c r="AQ1" s="74"/>
+    </row>
+    <row r="2" spans="1:43" ht="15">
       <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
@@ -2026,8 +2045,17 @@
       <c r="AN2" s="16" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:40">
+      <c r="AO2" s="73" t="s">
+        <v>238</v>
+      </c>
+      <c r="AP2" s="73" t="s">
+        <v>239</v>
+      </c>
+      <c r="AQ2" s="73" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43">
       <c r="A3" s="46" t="s">
         <v>183</v>
       </c>
@@ -2090,9 +2118,22 @@
         <v>0</v>
       </c>
       <c r="AM3" s="30"/>
-      <c r="AN3" s="30"/>
-    </row>
-    <row r="4" spans="1:40">
+      <c r="AN3" s="30">
+        <v>63</v>
+      </c>
+      <c r="AO3" s="75">
+        <f t="shared" ref="AO3:AO46" si="0">IF(AN3+AL3&gt;AQ3,AQ3,AN3+AL3)</f>
+        <v>63</v>
+      </c>
+      <c r="AP3" s="75">
+        <f t="shared" ref="AP3:AP8" si="1">IF(AN3+AL3&gt;AQ3,AL3+AN3-AQ3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43">
       <c r="A4" s="2" t="s">
         <v>71</v>
       </c>
@@ -2137,21 +2178,32 @@
       <c r="AH4" s="28"/>
       <c r="AI4" s="28"/>
       <c r="AJ4" s="30">
-        <f t="shared" ref="AJ4:AJ20" si="0">SUM(F4:AI4)</f>
+        <f t="shared" ref="AJ4:AJ20" si="2">SUM(F4:AI4)</f>
         <v>0</v>
       </c>
       <c r="AK4" s="30">
-        <f t="shared" ref="AK4:AK23" si="1">IF(AJ4&gt;100,AJ4-(AJ4-100),AJ4)</f>
+        <f t="shared" ref="AK4:AK23" si="3">IF(AJ4&gt;100,AJ4-(AJ4-100),AJ4)</f>
         <v>0</v>
       </c>
       <c r="AL4" s="30">
-        <f t="shared" ref="AL4:AL57" si="2">IF(AJ4&gt;100,(AJ4-100)/10,0)</f>
+        <f t="shared" ref="AL4:AL57" si="4">IF(AJ4&gt;100,(AJ4-100)/10,0)</f>
         <v>0</v>
       </c>
       <c r="AM4" s="30"/>
       <c r="AN4" s="30"/>
-    </row>
-    <row r="5" spans="1:40">
+      <c r="AO4" s="75">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AP4" s="75">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43">
       <c r="A5" s="18" t="s">
         <v>227</v>
       </c>
@@ -2200,21 +2252,34 @@
       <c r="AH5" s="28"/>
       <c r="AI5" s="28"/>
       <c r="AJ5" s="30">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="AK5" s="30">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="AL5" s="30">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM5" s="30"/>
+      <c r="AN5" s="30">
+        <v>68</v>
+      </c>
+      <c r="AO5" s="75">
         <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="AK5" s="30">
+        <v>68</v>
+      </c>
+      <c r="AP5" s="75">
         <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-      <c r="AL5" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AM5" s="30"/>
-      <c r="AN5" s="30"/>
-    </row>
-    <row r="6" spans="1:40">
+        <v>0</v>
+      </c>
+      <c r="AQ5" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43">
       <c r="A6" s="18" t="s">
         <v>219</v>
       </c>
@@ -2263,21 +2328,34 @@
       <c r="AH6" s="28"/>
       <c r="AI6" s="28"/>
       <c r="AJ6" s="30">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="AK6" s="30">
+        <f t="shared" si="3"/>
+        <v>90</v>
+      </c>
+      <c r="AL6" s="30">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM6" s="30"/>
+      <c r="AN6" s="30">
+        <v>71</v>
+      </c>
+      <c r="AO6" s="75">
         <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-      <c r="AK6" s="30">
+        <v>71</v>
+      </c>
+      <c r="AP6" s="75">
         <f t="shared" si="1"/>
-        <v>90</v>
-      </c>
-      <c r="AL6" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AM6" s="30"/>
-      <c r="AN6" s="30"/>
-    </row>
-    <row r="7" spans="1:40">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43">
       <c r="A7" s="2"/>
       <c r="B7" s="3" t="s">
         <v>74</v>
@@ -2326,21 +2404,34 @@
       <c r="AH7" s="28"/>
       <c r="AI7" s="28"/>
       <c r="AJ7" s="30">
+        <f t="shared" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="AK7" s="30">
+        <f t="shared" si="3"/>
+        <v>85</v>
+      </c>
+      <c r="AL7" s="30">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM7" s="30"/>
+      <c r="AN7" s="30">
+        <v>75</v>
+      </c>
+      <c r="AO7" s="75">
         <f t="shared" si="0"/>
-        <v>85</v>
-      </c>
-      <c r="AK7" s="30">
+        <v>75</v>
+      </c>
+      <c r="AP7" s="75">
         <f t="shared" si="1"/>
-        <v>85</v>
-      </c>
-      <c r="AL7" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AM7" s="30"/>
-      <c r="AN7" s="30"/>
-    </row>
-    <row r="8" spans="1:40">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43">
       <c r="A8" s="7" t="s">
         <v>76</v>
       </c>
@@ -2391,21 +2482,34 @@
       <c r="AH8" s="28"/>
       <c r="AI8" s="28"/>
       <c r="AJ8" s="30">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="AK8" s="30">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="AL8" s="30">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="AM8" s="30"/>
+      <c r="AN8" s="30">
+        <v>51</v>
+      </c>
+      <c r="AO8" s="75">
         <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-      <c r="AK8" s="30">
+        <v>53</v>
+      </c>
+      <c r="AP8" s="75">
         <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="AL8" s="30">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="AM8" s="30"/>
-      <c r="AN8" s="30"/>
-    </row>
-    <row r="9" spans="1:40">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43">
       <c r="A9" s="18" t="s">
         <v>222</v>
       </c>
@@ -2454,21 +2558,33 @@
       <c r="AH9" s="28"/>
       <c r="AI9" s="28"/>
       <c r="AJ9" s="30">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="AK9" s="30">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="AL9" s="30">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM9" s="30"/>
+      <c r="AN9" s="30">
+        <v>68</v>
+      </c>
+      <c r="AO9" s="75">
         <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="AK9" s="30">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="AL9" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AM9" s="30"/>
-      <c r="AN9" s="30"/>
-    </row>
-    <row r="10" spans="1:40">
+        <v>68</v>
+      </c>
+      <c r="AP9" s="75">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:43">
       <c r="A10" s="18" t="s">
         <v>80</v>
       </c>
@@ -2519,21 +2635,34 @@
       <c r="AH10" s="28"/>
       <c r="AI10" s="28"/>
       <c r="AJ10" s="30">
+        <f t="shared" si="2"/>
+        <v>105</v>
+      </c>
+      <c r="AK10" s="30">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="AL10" s="30">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="AM10" s="30"/>
+      <c r="AN10" s="30">
+        <v>62</v>
+      </c>
+      <c r="AO10" s="75">
         <f t="shared" si="0"/>
-        <v>105</v>
-      </c>
-      <c r="AK10" s="30">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="AL10" s="30">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="AM10" s="30"/>
-      <c r="AN10" s="30"/>
-    </row>
-    <row r="11" spans="1:40">
+        <v>62.5</v>
+      </c>
+      <c r="AP10" s="75">
+        <f t="shared" ref="AP10:AP46" si="5">IF(AN10+AL10&gt;AQ10,AL10+AN10-AQ10,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ10" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:43">
       <c r="A11" s="18"/>
       <c r="B11" s="18" t="s">
         <v>236</v>
@@ -2578,21 +2707,34 @@
       <c r="AH11" s="28"/>
       <c r="AI11" s="28"/>
       <c r="AJ11" s="30">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="AK11" s="30">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="AL11" s="30">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM11" s="30"/>
+      <c r="AN11" s="30">
+        <v>75</v>
+      </c>
+      <c r="AO11" s="75">
         <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="AK11" s="30">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="AL11" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AM11" s="30"/>
-      <c r="AN11" s="30"/>
-    </row>
-    <row r="12" spans="1:40">
+        <v>75</v>
+      </c>
+      <c r="AP11" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ11" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43">
       <c r="A12" s="18" t="s">
         <v>216</v>
       </c>
@@ -2639,21 +2781,34 @@
       <c r="AH12" s="28"/>
       <c r="AI12" s="28"/>
       <c r="AJ12" s="30">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="AK12" s="30">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="AL12" s="30">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM12" s="30"/>
+      <c r="AN12" s="30">
+        <v>65</v>
+      </c>
+      <c r="AO12" s="75">
         <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="AK12" s="30">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="AL12" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AM12" s="30"/>
-      <c r="AN12" s="30"/>
-    </row>
-    <row r="13" spans="1:40">
+        <v>65</v>
+      </c>
+      <c r="AP12" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ12" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43">
       <c r="A13" s="18" t="s">
         <v>178</v>
       </c>
@@ -2704,21 +2859,32 @@
       <c r="AH13" s="28"/>
       <c r="AI13" s="28"/>
       <c r="AJ13" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="AK13" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="AL13" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM13" s="30"/>
       <c r="AN13" s="30"/>
-    </row>
-    <row r="14" spans="1:40">
+      <c r="AO13" s="75">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AP13" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ13" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:43">
       <c r="A14" s="18" t="s">
         <v>192</v>
       </c>
@@ -2769,21 +2935,34 @@
       <c r="AH14" s="28"/>
       <c r="AI14" s="28"/>
       <c r="AJ14" s="30">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="AK14" s="30">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="AL14" s="30">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM14" s="30"/>
+      <c r="AN14" s="30">
+        <v>68</v>
+      </c>
+      <c r="AO14" s="75">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="AK14" s="30">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="AL14" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AM14" s="30"/>
-      <c r="AN14" s="30"/>
-    </row>
-    <row r="15" spans="1:40">
+        <v>68</v>
+      </c>
+      <c r="AP14" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ14" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:43">
       <c r="A15" s="2" t="s">
         <v>83</v>
       </c>
@@ -2830,21 +3009,34 @@
       <c r="AH15" s="28"/>
       <c r="AI15" s="28"/>
       <c r="AJ15" s="30">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="AK15" s="30">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="AL15" s="30">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM15" s="30"/>
+      <c r="AN15" s="30">
+        <v>53</v>
+      </c>
+      <c r="AO15" s="75">
         <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="AK15" s="30">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="AL15" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AM15" s="30"/>
-      <c r="AN15" s="30"/>
-    </row>
-    <row r="16" spans="1:40">
+        <v>53</v>
+      </c>
+      <c r="AP15" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ15" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43">
       <c r="A16" s="18" t="s">
         <v>205</v>
       </c>
@@ -2891,21 +3083,34 @@
       <c r="AH16" s="28"/>
       <c r="AI16" s="28"/>
       <c r="AJ16" s="30">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="AK16" s="30">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="AL16" s="30">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM16" s="30"/>
+      <c r="AN16" s="30">
+        <v>73</v>
+      </c>
+      <c r="AO16" s="75">
         <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="AK16" s="30">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="AL16" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AM16" s="30"/>
-      <c r="AN16" s="30"/>
-    </row>
-    <row r="17" spans="1:40">
+        <v>73</v>
+      </c>
+      <c r="AP16" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ16" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:43">
       <c r="A17" s="18" t="s">
         <v>195</v>
       </c>
@@ -2956,21 +3161,34 @@
       <c r="AH17" s="28"/>
       <c r="AI17" s="28"/>
       <c r="AJ17" s="30">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
+      <c r="AK17" s="30">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="AL17" s="30">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AM17" s="30"/>
+      <c r="AN17" s="30">
+        <v>75</v>
+      </c>
+      <c r="AO17" s="75">
         <f t="shared" si="0"/>
-        <v>110</v>
-      </c>
-      <c r="AK17" s="30">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="AL17" s="30">
-        <f t="shared" si="2"/>
+        <v>75</v>
+      </c>
+      <c r="AP17" s="75">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="AM17" s="30"/>
-      <c r="AN17" s="30"/>
-    </row>
-    <row r="18" spans="1:40">
+      <c r="AQ17" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:43">
       <c r="A18" s="2" t="s">
         <v>86</v>
       </c>
@@ -3019,21 +3237,34 @@
       <c r="AH18" s="28"/>
       <c r="AI18" s="28"/>
       <c r="AJ18" s="30">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="AK18" s="30">
+        <f t="shared" si="3"/>
+        <v>80</v>
+      </c>
+      <c r="AL18" s="30">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM18" s="30"/>
+      <c r="AN18" s="30">
+        <v>68</v>
+      </c>
+      <c r="AO18" s="75">
         <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="AK18" s="30">
-        <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="AL18" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AM18" s="30"/>
-      <c r="AN18" s="30"/>
-    </row>
-    <row r="19" spans="1:40">
+        <v>68</v>
+      </c>
+      <c r="AP18" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ18" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:43">
       <c r="A19" s="18" t="s">
         <v>212</v>
       </c>
@@ -3080,21 +3311,34 @@
       <c r="AH19" s="28"/>
       <c r="AI19" s="28"/>
       <c r="AJ19" s="30">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="AK19" s="30">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="AL19" s="30">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM19" s="30"/>
+      <c r="AN19" s="30">
+        <v>56</v>
+      </c>
+      <c r="AO19" s="75">
         <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="AK19" s="30">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="AL19" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AM19" s="30"/>
-      <c r="AN19" s="30"/>
-    </row>
-    <row r="20" spans="1:40">
+        <v>56</v>
+      </c>
+      <c r="AP19" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ19" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:43">
       <c r="A20" s="18" t="s">
         <v>89</v>
       </c>
@@ -3145,21 +3389,34 @@
       <c r="AH20" s="28"/>
       <c r="AI20" s="28"/>
       <c r="AJ20" s="30">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="AK20" s="30">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="AL20" s="30">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AM20" s="30"/>
+      <c r="AN20" s="30">
+        <v>65</v>
+      </c>
+      <c r="AO20" s="75">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="AK20" s="30">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="AL20" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AM20" s="30"/>
-      <c r="AN20" s="30"/>
-    </row>
-    <row r="21" spans="1:40">
+        <v>65</v>
+      </c>
+      <c r="AP20" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ20" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:43">
       <c r="A21" s="18" t="s">
         <v>202</v>
       </c>
@@ -3212,17 +3469,30 @@
         <v>80</v>
       </c>
       <c r="AK21" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
       <c r="AL21" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM21" s="30"/>
-      <c r="AN21" s="30"/>
-    </row>
-    <row r="22" spans="1:40">
+      <c r="AN21" s="30">
+        <v>75</v>
+      </c>
+      <c r="AO21" s="75">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="AP21" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ21" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:43">
       <c r="A22" s="2" t="s">
         <v>92</v>
       </c>
@@ -3273,21 +3543,34 @@
       <c r="AH22" s="28"/>
       <c r="AI22" s="28"/>
       <c r="AJ22" s="30">
-        <f t="shared" ref="AJ22:AJ23" si="3">SUM(F22:AI22)</f>
+        <f t="shared" ref="AJ22:AJ23" si="6">SUM(F22:AI22)</f>
         <v>85</v>
       </c>
       <c r="AK22" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>85</v>
       </c>
       <c r="AL22" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM22" s="30"/>
-      <c r="AN22" s="30"/>
-    </row>
-    <row r="23" spans="1:40">
+      <c r="AN22" s="30">
+        <v>65</v>
+      </c>
+      <c r="AO22" s="75">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="AP22" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ22" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:43">
       <c r="A23" s="2" t="s">
         <v>96</v>
       </c>
@@ -3338,21 +3621,34 @@
       <c r="AH23" s="28"/>
       <c r="AI23" s="28"/>
       <c r="AJ23" s="30">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+      <c r="AK23" s="30">
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="AK23" s="30">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
       <c r="AL23" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM23" s="30"/>
-      <c r="AN23" s="30"/>
-    </row>
-    <row r="24" spans="1:40">
+      <c r="AN23" s="30">
+        <v>75</v>
+      </c>
+      <c r="AO23" s="75">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="AP23" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ23" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:43">
       <c r="A24" s="2" t="s">
         <v>99</v>
       </c>
@@ -3399,21 +3695,34 @@
       <c r="AH24" s="28"/>
       <c r="AI24" s="28"/>
       <c r="AJ24" s="30">
-        <f t="shared" ref="AJ24:AJ34" si="4">SUM(F24:AI24)</f>
+        <f t="shared" ref="AJ24:AJ34" si="7">SUM(F24:AI24)</f>
         <v>50</v>
       </c>
       <c r="AK24" s="30">
-        <f t="shared" ref="AK24:AK34" si="5">IF(AJ24&gt;100,AJ24-(AJ24-100),AJ24)</f>
+        <f t="shared" ref="AK24:AK34" si="8">IF(AJ24&gt;100,AJ24-(AJ24-100),AJ24)</f>
         <v>50</v>
       </c>
       <c r="AL24" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM24" s="30"/>
-      <c r="AN24" s="30"/>
-    </row>
-    <row r="25" spans="1:40">
+      <c r="AN24" s="30">
+        <v>65</v>
+      </c>
+      <c r="AO24" s="75">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="AP24" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ24" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:43">
       <c r="A25" s="6" t="s">
         <v>102</v>
       </c>
@@ -3462,21 +3771,34 @@
       <c r="AH25" s="28"/>
       <c r="AI25" s="28"/>
       <c r="AJ25" s="30">
+        <f t="shared" si="7"/>
+        <v>70</v>
+      </c>
+      <c r="AK25" s="30">
+        <f t="shared" si="8"/>
+        <v>70</v>
+      </c>
+      <c r="AL25" s="30">
         <f t="shared" si="4"/>
-        <v>70</v>
-      </c>
-      <c r="AK25" s="30">
+        <v>0</v>
+      </c>
+      <c r="AM25" s="30"/>
+      <c r="AN25" s="30">
+        <v>49</v>
+      </c>
+      <c r="AO25" s="75">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="AP25" s="75">
         <f t="shared" si="5"/>
-        <v>70</v>
-      </c>
-      <c r="AL25" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AM25" s="30"/>
-      <c r="AN25" s="30"/>
-    </row>
-    <row r="26" spans="1:40">
+        <v>0</v>
+      </c>
+      <c r="AQ25" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:43">
       <c r="A26" s="18" t="s">
         <v>105</v>
       </c>
@@ -3527,21 +3849,34 @@
       <c r="AH26" s="28"/>
       <c r="AI26" s="28"/>
       <c r="AJ26" s="30">
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+      <c r="AK26" s="30">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="AL26" s="30">
         <f t="shared" si="4"/>
-        <v>100</v>
-      </c>
-      <c r="AK26" s="30">
+        <v>0</v>
+      </c>
+      <c r="AM26" s="30"/>
+      <c r="AN26" s="30">
+        <v>65</v>
+      </c>
+      <c r="AO26" s="75">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="AP26" s="75">
         <f t="shared" si="5"/>
-        <v>100</v>
-      </c>
-      <c r="AL26" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AM26" s="30"/>
-      <c r="AN26" s="30"/>
-    </row>
-    <row r="27" spans="1:40">
+        <v>0</v>
+      </c>
+      <c r="AQ26" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:43">
       <c r="A27" s="18" t="s">
         <v>68</v>
       </c>
@@ -3588,21 +3923,34 @@
       <c r="AH27" s="28"/>
       <c r="AI27" s="28"/>
       <c r="AJ27" s="30">
+        <f t="shared" si="7"/>
+        <v>50</v>
+      </c>
+      <c r="AK27" s="30">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="AL27" s="30">
         <f t="shared" si="4"/>
-        <v>50</v>
-      </c>
-      <c r="AK27" s="30">
+        <v>0</v>
+      </c>
+      <c r="AM27" s="30"/>
+      <c r="AN27" s="30">
+        <v>68</v>
+      </c>
+      <c r="AO27" s="75">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="AP27" s="75">
         <f t="shared" si="5"/>
-        <v>50</v>
-      </c>
-      <c r="AL27" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AM27" s="30"/>
-      <c r="AN27" s="30"/>
-    </row>
-    <row r="28" spans="1:40">
+        <v>0</v>
+      </c>
+      <c r="AQ27" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:43">
       <c r="A28" s="2" t="s">
         <v>108</v>
       </c>
@@ -3651,21 +3999,34 @@
       <c r="AH28" s="28"/>
       <c r="AI28" s="28"/>
       <c r="AJ28" s="30">
+        <f t="shared" si="7"/>
+        <v>70</v>
+      </c>
+      <c r="AK28" s="30">
+        <f t="shared" si="8"/>
+        <v>70</v>
+      </c>
+      <c r="AL28" s="30">
         <f t="shared" si="4"/>
-        <v>70</v>
-      </c>
-      <c r="AK28" s="30">
+        <v>0</v>
+      </c>
+      <c r="AM28" s="30"/>
+      <c r="AN28" s="30">
+        <v>65</v>
+      </c>
+      <c r="AO28" s="75">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="AP28" s="75">
         <f t="shared" si="5"/>
-        <v>70</v>
-      </c>
-      <c r="AL28" s="30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AM28" s="30"/>
-      <c r="AN28" s="30"/>
-    </row>
-    <row r="29" spans="1:40">
+        <v>0</v>
+      </c>
+      <c r="AQ28" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:43">
       <c r="A29" s="2" t="s">
         <v>111</v>
       </c>
@@ -3710,21 +4071,32 @@
       <c r="AH29" s="28"/>
       <c r="AI29" s="28"/>
       <c r="AJ29" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AK29" s="30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AL29" s="30">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AK29" s="30">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AL29" s="30">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AM29" s="30"/>
       <c r="AN29" s="30"/>
-    </row>
-    <row r="30" spans="1:40">
+      <c r="AO29" s="75">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AP29" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ29" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:43">
       <c r="A30" s="2" t="s">
         <v>114</v>
       </c>
@@ -3777,21 +4149,34 @@
       <c r="AH30" s="28"/>
       <c r="AI30" s="28"/>
       <c r="AJ30" s="30">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="AK30" s="30">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="AL30" s="30">
         <f t="shared" si="4"/>
-        <v>150</v>
-      </c>
-      <c r="AK30" s="30">
+        <v>5</v>
+      </c>
+      <c r="AM30" s="30"/>
+      <c r="AN30" s="30">
+        <v>68</v>
+      </c>
+      <c r="AO30" s="75">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="AP30" s="75">
         <f t="shared" si="5"/>
-        <v>100</v>
-      </c>
-      <c r="AL30" s="30">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="AM30" s="30"/>
-      <c r="AN30" s="30"/>
-    </row>
-    <row r="31" spans="1:40">
+        <v>0</v>
+      </c>
+      <c r="AQ30" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:43">
       <c r="A31" s="2" t="s">
         <v>117</v>
       </c>
@@ -3844,21 +4229,34 @@
       <c r="AH31" s="28"/>
       <c r="AI31" s="28"/>
       <c r="AJ31" s="30">
+        <f t="shared" si="7"/>
+        <v>170</v>
+      </c>
+      <c r="AK31" s="30">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="AL31" s="30">
         <f t="shared" si="4"/>
-        <v>170</v>
-      </c>
-      <c r="AK31" s="30">
+        <v>7</v>
+      </c>
+      <c r="AM31" s="30"/>
+      <c r="AN31" s="30">
+        <v>75</v>
+      </c>
+      <c r="AO31" s="75">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="AP31" s="75">
         <f t="shared" si="5"/>
-        <v>100</v>
-      </c>
-      <c r="AL31" s="30">
-        <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="AM31" s="30"/>
-      <c r="AN31" s="30"/>
-    </row>
-    <row r="32" spans="1:40">
+      <c r="AQ31" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:43">
       <c r="A32" s="2" t="s">
         <v>120</v>
       </c>
@@ -3909,21 +4307,34 @@
       <c r="AH32" s="28"/>
       <c r="AI32" s="28"/>
       <c r="AJ32" s="30">
+        <f t="shared" si="7"/>
+        <v>120</v>
+      </c>
+      <c r="AK32" s="30">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="AL32" s="30">
         <f t="shared" si="4"/>
-        <v>120</v>
-      </c>
-      <c r="AK32" s="30">
+        <v>2</v>
+      </c>
+      <c r="AM32" s="30"/>
+      <c r="AN32" s="30">
+        <v>53</v>
+      </c>
+      <c r="AO32" s="75">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="AP32" s="75">
         <f t="shared" si="5"/>
-        <v>100</v>
-      </c>
-      <c r="AL32" s="30">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="AM32" s="30"/>
-      <c r="AN32" s="30"/>
-    </row>
-    <row r="33" spans="1:40">
+        <v>0</v>
+      </c>
+      <c r="AQ32" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:43">
       <c r="A33" s="18" t="s">
         <v>186</v>
       </c>
@@ -3974,21 +4385,34 @@
       <c r="AH33" s="28"/>
       <c r="AI33" s="28"/>
       <c r="AJ33" s="30">
+        <f t="shared" si="7"/>
+        <v>110</v>
+      </c>
+      <c r="AK33" s="30">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="AL33" s="30">
         <f t="shared" si="4"/>
-        <v>110</v>
-      </c>
-      <c r="AK33" s="30">
+        <v>1</v>
+      </c>
+      <c r="AM33" s="30"/>
+      <c r="AN33" s="30">
+        <v>58</v>
+      </c>
+      <c r="AO33" s="75">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="AP33" s="75">
         <f t="shared" si="5"/>
-        <v>100</v>
-      </c>
-      <c r="AL33" s="30">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AM33" s="30"/>
-      <c r="AN33" s="30"/>
-    </row>
-    <row r="34" spans="1:40">
+        <v>0</v>
+      </c>
+      <c r="AQ33" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:43">
       <c r="A34" s="2" t="s">
         <v>123</v>
       </c>
@@ -4039,21 +4463,32 @@
       <c r="AH34" s="28"/>
       <c r="AI34" s="28"/>
       <c r="AJ34" s="30">
+        <f t="shared" si="7"/>
+        <v>105</v>
+      </c>
+      <c r="AK34" s="30">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="AL34" s="30">
         <f t="shared" si="4"/>
-        <v>105</v>
-      </c>
-      <c r="AK34" s="30">
-        <f t="shared" si="5"/>
-        <v>100</v>
-      </c>
-      <c r="AL34" s="30">
-        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="AM34" s="30"/>
       <c r="AN34" s="30"/>
-    </row>
-    <row r="35" spans="1:40">
+      <c r="AO34" s="75">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="AP34" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ34" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:43">
       <c r="A35" s="2" t="s">
         <v>126</v>
       </c>
@@ -4104,21 +4539,34 @@
       <c r="AH35" s="28"/>
       <c r="AI35" s="28"/>
       <c r="AJ35" s="30">
-        <f t="shared" ref="AJ35:AJ61" si="6">SUM(F35:AI35)</f>
+        <f t="shared" ref="AJ35:AJ61" si="9">SUM(F35:AI35)</f>
         <v>85</v>
       </c>
       <c r="AK35" s="30">
-        <f t="shared" ref="AK35:AK61" si="7">IF(AJ35&gt;100,AJ35-(AJ35-100),AJ35)</f>
+        <f t="shared" ref="AK35:AK61" si="10">IF(AJ35&gt;100,AJ35-(AJ35-100),AJ35)</f>
         <v>85</v>
       </c>
       <c r="AL35" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM35" s="30"/>
-      <c r="AN35" s="30"/>
-    </row>
-    <row r="36" spans="1:40">
+      <c r="AN35" s="30">
+        <v>68</v>
+      </c>
+      <c r="AO35" s="75">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="AP35" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ35" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:43">
       <c r="A36" s="18" t="s">
         <v>209</v>
       </c>
@@ -4167,21 +4615,34 @@
       <c r="AH36" s="28"/>
       <c r="AI36" s="28"/>
       <c r="AJ36" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>70</v>
       </c>
       <c r="AK36" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>70</v>
       </c>
       <c r="AL36" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM36" s="30"/>
-      <c r="AN36" s="30"/>
-    </row>
-    <row r="37" spans="1:40">
+      <c r="AN36" s="30">
+        <v>70</v>
+      </c>
+      <c r="AO36" s="75">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="AP36" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ36" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:43">
       <c r="A37" s="2" t="s">
         <v>130</v>
       </c>
@@ -4232,21 +4693,34 @@
       <c r="AH37" s="28"/>
       <c r="AI37" s="28"/>
       <c r="AJ37" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>120</v>
       </c>
       <c r="AK37" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>100</v>
       </c>
       <c r="AL37" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AM37" s="30"/>
-      <c r="AN37" s="30"/>
-    </row>
-    <row r="38" spans="1:40">
+      <c r="AN37" s="30">
+        <v>68</v>
+      </c>
+      <c r="AO37" s="75">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="AP37" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ37" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:43">
       <c r="A38" s="7" t="s">
         <v>233</v>
       </c>
@@ -4297,21 +4771,34 @@
       <c r="AH38" s="28"/>
       <c r="AI38" s="28"/>
       <c r="AJ38" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>130</v>
       </c>
       <c r="AK38" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>100</v>
       </c>
       <c r="AL38" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="AM38" s="30"/>
-      <c r="AN38" s="30"/>
-    </row>
-    <row r="39" spans="1:40">
+      <c r="AN38" s="30">
+        <v>56</v>
+      </c>
+      <c r="AO38" s="75">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="AP38" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ38" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:43">
       <c r="A39" s="18" t="s">
         <v>135</v>
       </c>
@@ -4362,21 +4849,32 @@
       <c r="AH39" s="28"/>
       <c r="AI39" s="28"/>
       <c r="AJ39" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="AK39" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>100</v>
       </c>
       <c r="AL39" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM39" s="30"/>
       <c r="AN39" s="30"/>
-    </row>
-    <row r="40" spans="1:40">
+      <c r="AO39" s="75">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AP39" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ39" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:43">
       <c r="A40" s="18" t="s">
         <v>230</v>
       </c>
@@ -4425,21 +4923,34 @@
       <c r="AH40" s="28"/>
       <c r="AI40" s="28"/>
       <c r="AJ40" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>110</v>
       </c>
       <c r="AK40" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>100</v>
       </c>
       <c r="AL40" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AM40" s="30"/>
-      <c r="AN40" s="30"/>
-    </row>
-    <row r="41" spans="1:40">
+      <c r="AN40" s="30">
+        <v>2</v>
+      </c>
+      <c r="AO40" s="75">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AP40" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ40" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:43">
       <c r="A41" s="2" t="s">
         <v>138</v>
       </c>
@@ -4490,21 +5001,34 @@
       <c r="AH41" s="28"/>
       <c r="AI41" s="28"/>
       <c r="AJ41" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>85</v>
       </c>
       <c r="AK41" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>85</v>
       </c>
       <c r="AL41" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM41" s="30"/>
-      <c r="AN41" s="30"/>
-    </row>
-    <row r="42" spans="1:40">
+      <c r="AN41" s="30">
+        <v>75</v>
+      </c>
+      <c r="AO41" s="75">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="AP41" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ41" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:43">
       <c r="A42" s="18" t="s">
         <v>198</v>
       </c>
@@ -4549,21 +5073,32 @@
       <c r="AH42" s="28"/>
       <c r="AI42" s="28"/>
       <c r="AJ42" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AK42" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AL42" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM42" s="30"/>
       <c r="AN42" s="30"/>
-    </row>
-    <row r="43" spans="1:40">
+      <c r="AO42" s="75">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AP42" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ42" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:43">
       <c r="A43" s="18" t="s">
         <v>141</v>
       </c>
@@ -4612,21 +5147,34 @@
       <c r="AH43" s="28"/>
       <c r="AI43" s="28"/>
       <c r="AJ43" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>90</v>
       </c>
       <c r="AK43" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>90</v>
       </c>
       <c r="AL43" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM43" s="30"/>
-      <c r="AN43" s="30"/>
-    </row>
-    <row r="44" spans="1:40">
+      <c r="AN43" s="30">
+        <v>60</v>
+      </c>
+      <c r="AO43" s="75">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="AP43" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ43" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:43">
       <c r="A44" s="18" t="s">
         <v>144</v>
       </c>
@@ -4677,21 +5225,34 @@
       <c r="AH44" s="28"/>
       <c r="AI44" s="28"/>
       <c r="AJ44" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>120</v>
       </c>
       <c r="AK44" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>100</v>
       </c>
       <c r="AL44" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AM44" s="30"/>
-      <c r="AN44" s="30"/>
-    </row>
-    <row r="45" spans="1:40">
+      <c r="AN44" s="30">
+        <v>67</v>
+      </c>
+      <c r="AO44" s="75">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="AP44" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ44" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:43">
       <c r="A45" s="2" t="s">
         <v>147</v>
       </c>
@@ -4742,21 +5303,34 @@
       <c r="AH45" s="28"/>
       <c r="AI45" s="28"/>
       <c r="AJ45" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>120</v>
       </c>
       <c r="AK45" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>100</v>
       </c>
       <c r="AL45" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AM45" s="30"/>
-      <c r="AN45" s="30"/>
-    </row>
-    <row r="46" spans="1:40">
+      <c r="AN45" s="30">
+        <v>70</v>
+      </c>
+      <c r="AO45" s="75">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="AP45" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ45" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:43">
       <c r="A46" s="18" t="s">
         <v>150</v>
       </c>
@@ -4805,21 +5379,34 @@
       <c r="AH46" s="28"/>
       <c r="AI46" s="28"/>
       <c r="AJ46" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>90</v>
       </c>
       <c r="AK46" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>90</v>
       </c>
       <c r="AL46" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM46" s="30"/>
-      <c r="AN46" s="30"/>
-    </row>
-    <row r="47" spans="1:40">
+      <c r="AN46" s="30">
+        <v>68</v>
+      </c>
+      <c r="AO46" s="75">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="AP46" s="75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ46" s="73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:43">
       <c r="A47" s="2" t="s">
         <v>153</v>
       </c>
@@ -4870,21 +5457,32 @@
       <c r="AH47" s="28"/>
       <c r="AI47" s="28"/>
       <c r="AJ47" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>110</v>
       </c>
       <c r="AK47" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>100</v>
       </c>
       <c r="AL47" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AM47" s="30"/>
       <c r="AN47" s="30"/>
-    </row>
-    <row r="48" spans="1:40">
+      <c r="AO47" s="75">
+        <f t="shared" ref="AO47:AO62" si="11">IF(AN47+AL47&gt;AQ47,AQ47,AN47+AL47)</f>
+        <v>1</v>
+      </c>
+      <c r="AP47" s="75">
+        <f t="shared" ref="AP47:AP62" si="12">IF(AN47+AL47&gt;AQ47,AL47+AN47-AQ47,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ47" s="73">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:43">
       <c r="A48" s="2" t="s">
         <v>156</v>
       </c>
@@ -4933,21 +5531,34 @@
       <c r="AH48" s="28"/>
       <c r="AI48" s="28"/>
       <c r="AJ48" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>70</v>
       </c>
       <c r="AK48" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>70</v>
       </c>
       <c r="AL48" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM48" s="30"/>
-      <c r="AN48" s="30"/>
-    </row>
-    <row r="49" spans="1:40">
+      <c r="AN48" s="30">
+        <v>18</v>
+      </c>
+      <c r="AO48" s="75">
+        <f t="shared" si="11"/>
+        <v>18</v>
+      </c>
+      <c r="AP48" s="75">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AQ48" s="73">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:43">
       <c r="A49" s="2" t="s">
         <v>159</v>
       </c>
@@ -5000,21 +5611,34 @@
       <c r="AH49" s="28"/>
       <c r="AI49" s="28"/>
       <c r="AJ49" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>170</v>
       </c>
       <c r="AK49" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>100</v>
       </c>
       <c r="AL49" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="AM49" s="30"/>
-      <c r="AN49" s="30"/>
-    </row>
-    <row r="50" spans="1:40">
+      <c r="AN49" s="30">
+        <v>75</v>
+      </c>
+      <c r="AO49" s="75">
+        <f t="shared" si="11"/>
+        <v>78</v>
+      </c>
+      <c r="AP49" s="75">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="AQ49" s="73">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:43">
       <c r="A50" s="18" t="s">
         <v>189</v>
       </c>
@@ -5061,21 +5685,34 @@
       <c r="AH50" s="28"/>
       <c r="AI50" s="28"/>
       <c r="AJ50" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>70</v>
       </c>
       <c r="AK50" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>70</v>
       </c>
       <c r="AL50" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM50" s="30"/>
-      <c r="AN50" s="30"/>
-    </row>
-    <row r="51" spans="1:40">
+      <c r="AN50" s="30">
+        <v>55</v>
+      </c>
+      <c r="AO50" s="75">
+        <f t="shared" si="11"/>
+        <v>55</v>
+      </c>
+      <c r="AP50" s="75">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AQ50" s="73">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:43">
       <c r="A51" s="2" t="s">
         <v>162</v>
       </c>
@@ -5122,21 +5759,34 @@
       <c r="AH51" s="28"/>
       <c r="AI51" s="28"/>
       <c r="AJ51" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>50</v>
       </c>
       <c r="AK51" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>50</v>
       </c>
       <c r="AL51" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM51" s="30"/>
-      <c r="AN51" s="30"/>
-    </row>
-    <row r="52" spans="1:40">
+      <c r="AN51" s="30">
+        <v>65</v>
+      </c>
+      <c r="AO51" s="75">
+        <f t="shared" si="11"/>
+        <v>65</v>
+      </c>
+      <c r="AP51" s="75">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AQ51" s="73">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:43">
       <c r="A52" s="18" t="s">
         <v>166</v>
       </c>
@@ -5187,21 +5837,34 @@
       <c r="AH52" s="28"/>
       <c r="AI52" s="28"/>
       <c r="AJ52" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>95</v>
       </c>
       <c r="AK52" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>95</v>
       </c>
       <c r="AL52" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM52" s="30"/>
-      <c r="AN52" s="30"/>
-    </row>
-    <row r="53" spans="1:40">
+      <c r="AN52" s="30">
+        <v>64</v>
+      </c>
+      <c r="AO52" s="75">
+        <f t="shared" si="11"/>
+        <v>64</v>
+      </c>
+      <c r="AP52" s="75">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AQ52" s="73">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:43">
       <c r="A53" s="18" t="s">
         <v>225</v>
       </c>
@@ -5250,21 +5913,34 @@
       <c r="AH53" s="28"/>
       <c r="AI53" s="28"/>
       <c r="AJ53" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>70</v>
       </c>
       <c r="AK53" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>70</v>
       </c>
       <c r="AL53" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM53" s="30"/>
-      <c r="AN53" s="30"/>
-    </row>
-    <row r="54" spans="1:40">
+      <c r="AN53" s="30">
+        <v>68</v>
+      </c>
+      <c r="AO53" s="75">
+        <f t="shared" si="11"/>
+        <v>68</v>
+      </c>
+      <c r="AP53" s="75">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AQ53" s="73">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:43">
       <c r="A54" s="18" t="s">
         <v>169</v>
       </c>
@@ -5315,21 +5991,34 @@
       <c r="AH54" s="28"/>
       <c r="AI54" s="28"/>
       <c r="AJ54" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>130</v>
       </c>
       <c r="AK54" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>100</v>
       </c>
       <c r="AL54" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="AM54" s="30"/>
-      <c r="AN54" s="30"/>
-    </row>
-    <row r="55" spans="1:40">
+      <c r="AN54" s="30">
+        <v>75</v>
+      </c>
+      <c r="AO54" s="75">
+        <f t="shared" si="11"/>
+        <v>78</v>
+      </c>
+      <c r="AP54" s="75">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AQ54" s="73">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="1:43">
       <c r="A55" s="18" t="s">
         <v>172</v>
       </c>
@@ -5380,21 +6069,34 @@
       <c r="AH55" s="28"/>
       <c r="AI55" s="28"/>
       <c r="AJ55" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>130</v>
       </c>
       <c r="AK55" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>100</v>
       </c>
       <c r="AL55" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="AM55" s="30"/>
-      <c r="AN55" s="30"/>
-    </row>
-    <row r="56" spans="1:40">
+      <c r="AN55" s="30">
+        <v>75</v>
+      </c>
+      <c r="AO55" s="75">
+        <f t="shared" si="11"/>
+        <v>78</v>
+      </c>
+      <c r="AP55" s="75">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AQ55" s="73">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" spans="1:43">
       <c r="A56" s="18" t="s">
         <v>172</v>
       </c>
@@ -5445,21 +6147,34 @@
       <c r="AH56" s="28"/>
       <c r="AI56" s="28"/>
       <c r="AJ56" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>130</v>
       </c>
       <c r="AK56" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>100</v>
       </c>
       <c r="AL56" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="AM56" s="30"/>
-      <c r="AN56" s="30"/>
-    </row>
-    <row r="57" spans="1:40">
+      <c r="AN56" s="30">
+        <v>75</v>
+      </c>
+      <c r="AO56" s="75">
+        <f t="shared" si="11"/>
+        <v>78</v>
+      </c>
+      <c r="AP56" s="75">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AQ56" s="73">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="57" spans="1:43">
       <c r="A57" s="18" t="s">
         <v>175</v>
       </c>
@@ -5508,21 +6223,34 @@
       <c r="AH57" s="28"/>
       <c r="AI57" s="28"/>
       <c r="AJ57" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>80</v>
       </c>
       <c r="AK57" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>80</v>
       </c>
       <c r="AL57" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM57" s="30"/>
-      <c r="AN57" s="30"/>
-    </row>
-    <row r="58" spans="1:40">
+      <c r="AN57" s="30">
+        <v>62</v>
+      </c>
+      <c r="AO57" s="75">
+        <f t="shared" si="11"/>
+        <v>62</v>
+      </c>
+      <c r="AP57" s="75">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AQ57" s="73">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="58" spans="1:43">
       <c r="A58" s="18"/>
       <c r="B58" s="19"/>
       <c r="C58" s="19"/>
@@ -5559,21 +6287,32 @@
       <c r="AH58" s="28"/>
       <c r="AI58" s="28"/>
       <c r="AJ58" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AK58" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AL58" s="30">
-        <f t="shared" ref="AL35:AL61" si="8">IF(AK58&gt;100,AK58-100,0)</f>
+        <f t="shared" ref="AL58:AL61" si="13">IF(AK58&gt;100,AK58-100,0)</f>
         <v>0</v>
       </c>
       <c r="AM58" s="30"/>
       <c r="AN58" s="30"/>
-    </row>
-    <row r="59" spans="1:40">
+      <c r="AO58" s="75">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AP58" s="75">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AQ58" s="73">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="59" spans="1:43">
       <c r="A59" s="18"/>
       <c r="B59" s="19"/>
       <c r="C59" s="19"/>
@@ -5610,21 +6349,32 @@
       <c r="AH59" s="28"/>
       <c r="AI59" s="28"/>
       <c r="AJ59" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AK59" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AL59" s="30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AM59" s="30"/>
       <c r="AN59" s="30"/>
-    </row>
-    <row r="60" spans="1:40">
+      <c r="AO59" s="75">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AP59" s="75">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AQ59" s="73">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="1:43">
       <c r="A60" s="18"/>
       <c r="B60" s="19"/>
       <c r="C60" s="19"/>
@@ -5661,21 +6411,32 @@
       <c r="AH60" s="28"/>
       <c r="AI60" s="28"/>
       <c r="AJ60" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AK60" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AL60" s="30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AM60" s="30"/>
       <c r="AN60" s="30"/>
-    </row>
-    <row r="61" spans="1:40">
+      <c r="AO60" s="75">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AP60" s="75">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AQ60" s="73">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="61" spans="1:43">
       <c r="A61" s="18"/>
       <c r="B61" s="19"/>
       <c r="C61" s="19"/>
@@ -5712,19 +6473,43 @@
       <c r="AH61" s="28"/>
       <c r="AI61" s="28"/>
       <c r="AJ61" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AK61" s="30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AL61" s="30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AM61" s="30"/>
       <c r="AN61" s="30"/>
+      <c r="AO61" s="75">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AP61" s="75">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AQ61" s="73">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="62" spans="1:43">
+      <c r="AO62" s="75">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AP62" s="75">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AQ62" s="73">
+        <v>91</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A3:O57">

</xml_diff>